<commit_message>
COVID-19 data in European countries
</commit_message>
<xml_diff>
--- a/Real-world data in Europe/Deaths.xlsx
+++ b/Real-world data in Europe/Deaths.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanyixuan/Desktop/CoronaProj/data and experiments/Europe data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanyixuan/Documents/GitHub/Statistical_Inference_Using_GLEaM_with_Spatial_Heterogeneity_and_Correlation/Real-world data in Europe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FE5404-F4CB-894F-8CEF-E4AA0A1B53D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FB52E0-F8E0-B141-8B96-0602567353AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40780" yWindow="500" windowWidth="33280" windowHeight="21100" xr2:uid="{0060F9A0-0FBE-CE4D-9531-934C41634E86}"/>
+    <workbookView xWindow="2380" yWindow="500" windowWidth="33280" windowHeight="21100" xr2:uid="{0060F9A0-0FBE-CE4D-9531-934C41634E86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,28 +131,25 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -161,7 +158,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -183,7 +180,13 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -502,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C296DDD0-56D7-BE48-8E95-79C4CD97E896}">
   <dimension ref="A1:L124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C81" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -560,16 +563,16 @@
       <c r="B2" s="2">
         <v>460</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="8">
         <v>260</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="7">
         <v>210</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="9">
         <v>642</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="9">
         <v>6481</v>
       </c>
       <c r="G2" s="3">
@@ -598,16 +601,16 @@
       <c r="B3" s="2">
         <v>475</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8">
         <v>262</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="7">
         <v>211</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="9">
         <v>649</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="9">
         <v>6575</v>
       </c>
       <c r="G3" s="3">
@@ -636,16 +639,16 @@
       <c r="B4" s="2">
         <v>484</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="8">
         <v>265</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="7">
         <v>211</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="9">
         <v>653</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="9">
         <v>6649</v>
       </c>
       <c r="G4" s="3">
@@ -674,16 +677,16 @@
       <c r="B5" s="2">
         <v>493</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="8">
         <v>268</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="7">
         <v>214</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="9">
         <v>657</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="9">
         <v>6692</v>
       </c>
       <c r="G5" s="3">
@@ -712,16 +715,16 @@
       <c r="B6" s="2">
         <v>503</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="8">
         <v>275</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="7">
         <v>215</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="9">
         <v>666</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="9">
         <v>6831</v>
       </c>
       <c r="G6" s="3">
@@ -750,16 +753,16 @@
       <c r="B7" s="2">
         <v>506</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="8">
         <v>279</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="7">
         <v>216</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="9">
         <v>670</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="9">
         <v>6996</v>
       </c>
       <c r="G7" s="3">
@@ -788,16 +791,16 @@
       <c r="B8" s="2">
         <v>514</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="8">
         <v>281</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="7">
         <v>217</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="9">
         <v>673</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="9">
         <v>7119</v>
       </c>
       <c r="G8" s="3">
@@ -826,16 +829,16 @@
       <c r="B9" s="2">
         <v>522</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
         <v>288</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="7">
         <v>218</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="9">
         <v>680</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="9">
         <v>7266</v>
       </c>
       <c r="G9" s="3">
@@ -864,16 +867,16 @@
       <c r="B10" s="2">
         <v>526</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="8">
         <v>289</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="7">
         <v>219</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="9">
         <v>683</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="9">
         <v>7369</v>
       </c>
       <c r="G10" s="3">
@@ -902,16 +905,16 @@
       <c r="B11" s="2">
         <v>529</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="8">
         <v>291</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="7">
         <v>219</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="9">
         <v>688</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="9">
         <v>7395</v>
       </c>
       <c r="G11" s="3">
@@ -940,16 +943,16 @@
       <c r="B12" s="2">
         <v>533</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="8">
         <v>291</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="7">
         <v>224</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="9">
         <v>695</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="9">
         <v>7417</v>
       </c>
       <c r="G12" s="3">
@@ -978,16 +981,16 @@
       <c r="B13" s="2">
         <v>527</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="8">
         <v>292</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="7">
         <v>228</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="9">
         <v>698</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="9">
         <v>7533</v>
       </c>
       <c r="G13" s="3">
@@ -1016,16 +1019,16 @@
       <c r="B14" s="2">
         <v>533</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="8">
         <v>294</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="7">
         <v>229</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="9">
         <v>701</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="9">
         <v>7634</v>
       </c>
       <c r="G14" s="3">
@@ -1054,16 +1057,16 @@
       <c r="B15" s="2">
         <v>537</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="8">
         <v>296</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="7">
         <v>232</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="9">
         <v>702</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="9">
         <v>7723</v>
       </c>
       <c r="G15" s="3">
@@ -1092,16 +1095,16 @@
       <c r="B16" s="2">
         <v>537</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="8">
         <v>296</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="7">
         <v>232</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="9">
         <v>705</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="9">
         <v>7824</v>
       </c>
       <c r="G16" s="3">
@@ -1130,16 +1133,16 @@
       <c r="B17" s="2">
         <v>543</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="8">
         <v>297</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="7">
         <v>232</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="9">
         <v>709</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="9">
         <v>7881</v>
       </c>
       <c r="G17" s="3">
@@ -1168,16 +1171,16 @@
       <c r="B18" s="2">
         <v>547</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="8">
         <v>299</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="7">
         <v>232</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="9">
         <v>709</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="9">
         <v>7914</v>
       </c>
       <c r="G18" s="3">
@@ -1206,16 +1209,16 @@
       <c r="B19" s="2">
         <v>548</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="8">
         <v>299</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="7">
         <v>233</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="9">
         <v>710</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="9">
         <v>7935</v>
       </c>
       <c r="G19" s="3">
@@ -1244,16 +1247,16 @@
       <c r="B20" s="2">
         <v>551</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="8">
         <v>301</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="7">
         <v>233</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="9">
         <v>712</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="9">
         <v>8007</v>
       </c>
       <c r="G20" s="3">
@@ -1282,16 +1285,16 @@
       <c r="B21" s="2">
         <v>554</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="8">
         <v>301</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="7">
         <v>234</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="9">
         <v>716</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="9">
         <v>8090</v>
       </c>
       <c r="G21" s="3">
@@ -1320,16 +1323,16 @@
       <c r="B22" s="2">
         <v>561</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="8">
         <v>302</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="7">
         <v>235</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="9">
         <v>717</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="9">
         <v>8147</v>
       </c>
       <c r="G22" s="3">
@@ -1358,16 +1361,16 @@
       <c r="B23" s="2">
         <v>561</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="8">
         <v>302</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="7">
         <v>235</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="9">
         <v>721</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="9">
         <v>8174</v>
       </c>
       <c r="G23" s="3">
@@ -1396,16 +1399,16 @@
       <c r="B24" s="2">
         <v>561</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="8">
         <v>303</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="7">
         <v>235</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="9">
         <v>724</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="9">
         <v>8216</v>
       </c>
       <c r="G24" s="3">
@@ -1434,16 +1437,16 @@
       <c r="B25" s="2">
         <v>562</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="8">
         <v>303</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="7">
         <v>235</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="9">
         <v>728</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="9">
         <v>8247</v>
       </c>
       <c r="G25" s="3">
@@ -1472,16 +1475,16 @@
       <c r="B26" s="2">
         <v>563</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="8">
         <v>303</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="7">
         <v>235</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="9">
         <v>729</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="9">
         <v>8257</v>
       </c>
       <c r="G26" s="3">
@@ -1510,16 +1513,16 @@
       <c r="B27" s="2">
         <v>563</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="8">
         <v>304</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="7">
         <v>235</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="9">
         <v>730</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="9">
         <v>8302</v>
       </c>
       <c r="G27" s="3">
@@ -1548,16 +1551,16 @@
       <c r="B28" s="2">
         <v>565</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="8">
         <v>304</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="7">
         <v>235</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="9">
         <v>732</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="9">
         <v>8349</v>
       </c>
       <c r="G28" s="3">
@@ -1586,16 +1589,16 @@
       <c r="B29" s="2">
         <v>568</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="8">
         <v>304</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="7">
         <v>236</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="9">
         <v>736</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="9">
         <v>8411</v>
       </c>
       <c r="G29" s="3">
@@ -1624,16 +1627,16 @@
       <c r="B30" s="2">
         <v>568</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="8">
         <v>304</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="7">
         <v>236</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="9">
         <v>737</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="9">
         <v>8450</v>
       </c>
       <c r="G30" s="3">
@@ -1662,16 +1665,16 @@
       <c r="B31" s="2">
         <v>571</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="8">
         <v>305</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="7">
         <v>236</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="9">
         <v>739</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="9">
         <v>8489</v>
       </c>
       <c r="G31" s="3">
@@ -1700,16 +1703,16 @@
       <c r="B32" s="2">
         <v>574</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="8">
         <v>305</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="7">
         <v>236</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="9">
         <v>741</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="9">
         <v>8500</v>
       </c>
       <c r="G32" s="3">
@@ -1738,16 +1741,16 @@
       <c r="B33" s="2">
         <v>576</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="8">
         <v>305</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="7">
         <v>236</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="9">
         <v>741</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="9">
         <v>8511</v>
       </c>
       <c r="G33" s="3">
@@ -1776,16 +1779,16 @@
       <c r="B34" s="2">
         <v>580</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="8">
         <v>305</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="7">
         <v>237</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="9">
         <v>745</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="9">
         <v>8522</v>
       </c>
       <c r="G34" s="3">
@@ -1814,16 +1817,16 @@
       <c r="B35" s="2">
         <v>580</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="8">
         <v>305</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="7">
         <v>237</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="9">
         <v>746</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="9">
         <v>8551</v>
       </c>
       <c r="G35" s="3">
@@ -1852,16 +1855,16 @@
       <c r="B36" s="2">
         <v>582</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="8">
         <v>305</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="7">
         <v>238</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="9">
         <v>749</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="9">
         <v>8581</v>
       </c>
       <c r="G36" s="3">
@@ -1890,16 +1893,16 @@
       <c r="B37" s="2">
         <v>586</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="8">
         <v>305</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="7">
         <v>238</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="9">
         <v>752</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="9">
         <v>8613</v>
       </c>
       <c r="G37" s="3">
@@ -1928,16 +1931,16 @@
       <c r="B38" s="2">
         <v>587</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="8">
         <v>305</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="7">
         <v>238</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="9">
         <v>756</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="9">
         <v>8646</v>
       </c>
       <c r="G38" s="3">
@@ -1966,16 +1969,16 @@
       <c r="B39" s="2">
         <v>589</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="8">
         <v>305</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="7">
         <v>238</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="9">
         <v>758</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="9">
         <v>8668</v>
       </c>
       <c r="G39" s="3">
@@ -2004,16 +2007,16 @@
       <c r="B40" s="2">
         <v>593</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="8">
         <v>305</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="7">
         <v>239</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="9">
         <v>759</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="9">
         <v>8674</v>
       </c>
       <c r="G40" s="3">
@@ -2042,16 +2045,16 @@
       <c r="B41" s="2">
         <v>593</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="8">
         <v>305</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="7">
         <v>239</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="9">
         <v>760</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="9">
         <v>8711</v>
       </c>
       <c r="G41" s="3">
@@ -2080,16 +2083,16 @@
       <c r="B42" s="2">
         <v>593</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="8">
         <v>305</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="7">
         <v>239</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="9">
         <v>763</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="9">
         <v>8729</v>
       </c>
       <c r="G42" s="3">
@@ -2118,16 +2121,16 @@
       <c r="B43" s="2">
         <v>593</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="8">
         <v>305</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="7">
         <v>242</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="9">
         <v>765</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F43" s="9">
         <v>8755</v>
       </c>
       <c r="G43" s="3">
@@ -2156,16 +2159,16 @@
       <c r="B44" s="2">
         <v>594</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="8">
         <v>305</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="7">
         <v>242</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44" s="9">
         <v>767</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F44" s="9">
         <v>8763</v>
       </c>
       <c r="G44" s="3">
@@ -2194,16 +2197,16 @@
       <c r="B45" s="2">
         <v>597</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="8">
         <v>305</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="7">
         <v>242</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="9">
         <v>768</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F45" s="9">
         <v>8781</v>
       </c>
       <c r="G45" s="3">
@@ -2232,16 +2235,16 @@
       <c r="B46" s="2">
         <v>597</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="8">
         <v>305</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="7">
         <v>242</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46" s="9">
         <v>770</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F46" s="9">
         <v>8787</v>
       </c>
       <c r="G46" s="3">
@@ -2270,16 +2273,16 @@
       <c r="B47" s="2">
         <v>598</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="8">
         <v>305</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="7">
         <v>242</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="9">
         <v>771</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="9">
         <v>8791</v>
       </c>
       <c r="G47" s="3">
@@ -2308,16 +2311,16 @@
       <c r="B48" s="2">
         <v>598</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="8">
         <v>305</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="7">
         <v>242</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48" s="9">
         <v>776</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F48" s="9">
         <v>8800</v>
       </c>
       <c r="G48" s="3">
@@ -2346,16 +2349,16 @@
       <c r="B49" s="2">
         <v>598</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="8">
         <v>305</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="7">
         <v>243</v>
       </c>
-      <c r="E49" s="7">
+      <c r="E49" s="9">
         <v>782</v>
       </c>
-      <c r="F49" s="7">
+      <c r="F49" s="9">
         <v>8830</v>
       </c>
       <c r="G49" s="3">
@@ -2384,16 +2387,16 @@
       <c r="B50" s="2">
         <v>600</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="8">
         <v>305</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="7">
         <v>244</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E50" s="9">
         <v>785</v>
       </c>
-      <c r="F50" s="7">
+      <c r="F50" s="9">
         <v>8856</v>
       </c>
       <c r="G50" s="3">
@@ -2422,16 +2425,16 @@
       <c r="B51" s="2">
         <v>600</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="8">
         <v>305</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="7">
         <v>244</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="9">
         <v>786</v>
       </c>
-      <c r="F51" s="7">
+      <c r="F51" s="9">
         <v>8872</v>
       </c>
       <c r="G51" s="3">
@@ -2460,16 +2463,16 @@
       <c r="B52" s="2">
         <v>600</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="8">
         <v>305</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="7">
         <v>244</v>
       </c>
-      <c r="E52" s="7">
+      <c r="E52" s="9">
         <v>786</v>
       </c>
-      <c r="F52" s="7">
+      <c r="F52" s="9">
         <v>8883</v>
       </c>
       <c r="G52" s="3">
@@ -2498,16 +2501,16 @@
       <c r="B53" s="2">
         <v>600</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="8">
         <v>306</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="7">
         <v>244</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E53" s="9">
         <v>788</v>
       </c>
-      <c r="F53" s="7">
+      <c r="F53" s="9">
         <v>8882</v>
       </c>
       <c r="G53" s="3">
@@ -2536,16 +2539,16 @@
       <c r="B54" s="2">
         <v>602</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="8">
         <v>307</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="7">
         <v>248</v>
       </c>
-      <c r="E54" s="7">
+      <c r="E54" s="9">
         <v>791</v>
       </c>
-      <c r="F54" s="7">
+      <c r="F54" s="9">
         <v>8885</v>
       </c>
       <c r="G54" s="3">
@@ -2574,16 +2577,16 @@
       <c r="B55" s="2">
         <v>603</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="8">
         <v>307</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="7">
         <v>248</v>
       </c>
-      <c r="E55" s="7">
+      <c r="E55" s="9">
         <v>793</v>
       </c>
-      <c r="F55" s="7">
+      <c r="F55" s="9">
         <v>8895</v>
       </c>
       <c r="G55" s="3">
@@ -2612,16 +2615,16 @@
       <c r="B56" s="2">
         <v>603</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56" s="8">
         <v>307</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="7">
         <v>249</v>
       </c>
-      <c r="E56" s="7">
+      <c r="E56" s="9">
         <v>796</v>
       </c>
-      <c r="F56" s="7">
+      <c r="F56" s="9">
         <v>8914</v>
       </c>
       <c r="G56" s="3">
@@ -2650,16 +2653,16 @@
       <c r="B57" s="2">
         <v>603</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="8">
         <v>308</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="7">
         <v>249</v>
       </c>
-      <c r="E57" s="7">
+      <c r="E57" s="9">
         <v>798</v>
       </c>
-      <c r="F57" s="7">
+      <c r="F57" s="9">
         <v>8927</v>
       </c>
       <c r="G57" s="3">
@@ -2688,16 +2691,16 @@
       <c r="B58" s="2">
         <v>604</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58" s="8">
         <v>308</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="7">
         <v>249</v>
       </c>
-      <c r="E58" s="7">
+      <c r="E58" s="9">
         <v>802</v>
       </c>
-      <c r="F58" s="7">
+      <c r="F58" s="9">
         <v>8948</v>
       </c>
       <c r="G58" s="3">
@@ -2726,16 +2729,16 @@
       <c r="B59" s="2">
         <v>604</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="8">
         <v>308</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="7">
         <v>249</v>
       </c>
-      <c r="E59" s="7">
+      <c r="E59" s="9">
         <v>804</v>
       </c>
-      <c r="F59" s="7">
+      <c r="F59" s="9">
         <v>8954</v>
       </c>
       <c r="G59" s="3">
@@ -2764,16 +2767,16 @@
       <c r="B60" s="2">
         <v>604</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C60" s="8">
         <v>308</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="7">
         <v>249</v>
       </c>
-      <c r="E60" s="7">
+      <c r="E60" s="9">
         <v>805</v>
       </c>
-      <c r="F60" s="7">
+      <c r="F60" s="9">
         <v>8957</v>
       </c>
       <c r="G60" s="3">
@@ -2802,16 +2805,16 @@
       <c r="B61" s="2">
         <v>605</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C61" s="8">
         <v>308</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="7">
         <v>249</v>
       </c>
-      <c r="E61" s="7">
+      <c r="E61" s="9">
         <v>808</v>
       </c>
-      <c r="F61" s="7">
+      <c r="F61" s="9">
         <v>8961</v>
       </c>
       <c r="G61" s="3">
@@ -2840,16 +2843,16 @@
       <c r="B62" s="2">
         <v>605</v>
       </c>
-      <c r="C62" s="7">
+      <c r="C62" s="8">
         <v>309</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="7">
         <v>250</v>
       </c>
-      <c r="E62" s="7">
+      <c r="E62" s="9">
         <v>810</v>
       </c>
-      <c r="F62" s="7">
+      <c r="F62" s="9">
         <v>8973</v>
       </c>
       <c r="G62" s="3">
@@ -2878,16 +2881,16 @@
       <c r="B63" s="2">
         <v>606</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="8">
         <v>309</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="7">
         <v>251</v>
       </c>
-      <c r="E63" s="7">
+      <c r="E63" s="9">
         <v>811</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F63" s="9">
         <v>8985</v>
       </c>
       <c r="G63" s="3">
@@ -2916,16 +2919,16 @@
       <c r="B64" s="2">
         <v>606</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64" s="8">
         <v>309</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64" s="7">
         <v>251</v>
       </c>
-      <c r="E64" s="7">
+      <c r="E64" s="9">
         <v>811</v>
       </c>
-      <c r="F64" s="7">
+      <c r="F64" s="9">
         <v>8994</v>
       </c>
       <c r="G64" s="3">
@@ -2954,16 +2957,16 @@
       <c r="B65" s="2">
         <v>606</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="8">
         <v>309</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65" s="7">
         <v>251</v>
       </c>
-      <c r="E65" s="7">
+      <c r="E65" s="9">
         <v>812</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F65" s="9">
         <v>9003</v>
       </c>
       <c r="G65" s="3">
@@ -2992,16 +2995,16 @@
       <c r="B66" s="2">
         <v>606</v>
       </c>
-      <c r="C66" s="7">
+      <c r="C66" s="8">
         <v>309</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66" s="7">
         <v>251</v>
       </c>
-      <c r="E66" s="7">
+      <c r="E66" s="9">
         <v>815</v>
       </c>
-      <c r="F66" s="7">
+      <c r="F66" s="9">
         <v>9010</v>
       </c>
       <c r="G66" s="3">
@@ -3030,16 +3033,16 @@
       <c r="B67" s="2">
         <v>606</v>
       </c>
-      <c r="C67" s="7">
+      <c r="C67" s="8">
         <v>309</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="7">
         <v>251</v>
       </c>
-      <c r="E67" s="7">
+      <c r="E67" s="9">
         <v>816</v>
       </c>
-      <c r="F67" s="7">
+      <c r="F67" s="9">
         <v>9012</v>
       </c>
       <c r="G67" s="3">
@@ -3068,16 +3071,16 @@
       <c r="B68" s="2">
         <v>607</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="8">
         <v>309</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="7">
         <v>251</v>
       </c>
-      <c r="E68" s="7">
+      <c r="E68" s="9">
         <v>819</v>
       </c>
-      <c r="F68" s="7">
+      <c r="F68" s="9">
         <v>9016</v>
       </c>
       <c r="G68" s="3">
@@ -3106,16 +3109,16 @@
       <c r="B69" s="2">
         <v>609</v>
       </c>
-      <c r="C69" s="7">
+      <c r="C69" s="8">
         <v>309</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69" s="7">
         <v>251</v>
       </c>
-      <c r="E69" s="7">
+      <c r="E69" s="9">
         <v>819</v>
       </c>
-      <c r="F69" s="7">
+      <c r="F69" s="9">
         <v>9024</v>
       </c>
       <c r="G69" s="3">
@@ -3144,16 +3147,16 @@
       <c r="B70" s="2">
         <v>609</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C70" s="8">
         <v>309</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D70" s="7">
         <v>251</v>
       </c>
-      <c r="E70" s="7">
+      <c r="E70" s="9">
         <v>820</v>
       </c>
-      <c r="F70" s="7">
+      <c r="F70" s="9">
         <v>9036</v>
       </c>
       <c r="G70" s="3">
@@ -3182,16 +3185,16 @@
       <c r="B71" s="2">
         <v>609</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="8">
         <v>309</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71" s="7">
         <v>252</v>
       </c>
-      <c r="E71" s="7">
+      <c r="E71" s="9">
         <v>820</v>
       </c>
-      <c r="F71" s="7">
+      <c r="F71" s="9">
         <v>9048</v>
       </c>
       <c r="G71" s="3">
@@ -3220,16 +3223,16 @@
       <c r="B72" s="2">
         <v>609</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="8">
         <v>309</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D72" s="7">
         <v>252</v>
       </c>
-      <c r="E72" s="7">
+      <c r="E72" s="9">
         <v>820</v>
       </c>
-      <c r="F72" s="7">
+      <c r="F72" s="9">
         <v>9054</v>
       </c>
       <c r="G72" s="3">
@@ -3258,16 +3261,16 @@
       <c r="B73" s="2">
         <v>609</v>
       </c>
-      <c r="C73" s="7">
+      <c r="C73" s="8">
         <v>309</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D73" s="7">
         <v>252</v>
       </c>
-      <c r="E73" s="7">
+      <c r="E73" s="9">
         <v>821</v>
       </c>
-      <c r="F73" s="7">
+      <c r="F73" s="9">
         <v>9060</v>
       </c>
       <c r="G73" s="3">
@@ -3296,16 +3299,16 @@
       <c r="B74" s="2">
         <v>609</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="8">
         <v>309</v>
       </c>
-      <c r="D74" s="2">
+      <c r="D74" s="7">
         <v>252</v>
       </c>
-      <c r="E74" s="7">
+      <c r="E74" s="9">
         <v>821</v>
       </c>
-      <c r="F74" s="7">
+      <c r="F74" s="9">
         <v>9063</v>
       </c>
       <c r="G74" s="3">
@@ -3334,16 +3337,16 @@
       <c r="B75" s="2">
         <v>610</v>
       </c>
-      <c r="C75" s="7">
+      <c r="C75" s="8">
         <v>309</v>
       </c>
-      <c r="D75" s="2">
+      <c r="D75" s="7">
         <v>253</v>
       </c>
-      <c r="E75" s="7">
+      <c r="E75" s="9">
         <v>824</v>
       </c>
-      <c r="F75" s="7">
+      <c r="F75" s="9">
         <v>9064</v>
       </c>
       <c r="G75" s="3">
@@ -3372,16 +3375,16 @@
       <c r="B76" s="2">
         <v>610</v>
       </c>
-      <c r="C76" s="7">
+      <c r="C76" s="8">
         <v>309</v>
       </c>
-      <c r="D76" s="2">
+      <c r="D76" s="7">
         <v>253</v>
       </c>
-      <c r="E76" s="7">
+      <c r="E76" s="9">
         <v>826</v>
       </c>
-      <c r="F76" s="7">
+      <c r="F76" s="9">
         <v>9068</v>
       </c>
       <c r="G76" s="3">
@@ -3410,16 +3413,16 @@
       <c r="B77" s="2">
         <v>610</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="8">
         <v>309</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D77" s="7">
         <v>253</v>
       </c>
-      <c r="E77" s="7">
+      <c r="E77" s="9">
         <v>828</v>
       </c>
-      <c r="F77" s="7">
+      <c r="F77" s="9">
         <v>9071</v>
       </c>
       <c r="G77" s="3">
@@ -3448,16 +3451,16 @@
       <c r="B78" s="2">
         <v>610</v>
       </c>
-      <c r="C78" s="7">
+      <c r="C78" s="8">
         <v>309</v>
       </c>
-      <c r="D78" s="2">
+      <c r="D78" s="7">
         <v>254</v>
       </c>
-      <c r="E78" s="7">
+      <c r="E78" s="9">
         <v>829</v>
       </c>
-      <c r="F78" s="7">
+      <c r="F78" s="9">
         <v>9078</v>
       </c>
       <c r="G78" s="3">
@@ -3486,16 +3489,16 @@
       <c r="B79" s="2">
         <v>611</v>
       </c>
-      <c r="C79" s="7">
+      <c r="C79" s="8">
         <v>309</v>
       </c>
-      <c r="D79" s="2">
+      <c r="D79" s="7">
         <v>255</v>
       </c>
-      <c r="E79" s="7">
+      <c r="E79" s="9">
         <v>830</v>
       </c>
-      <c r="F79" s="7">
+      <c r="F79" s="9">
         <v>9082</v>
       </c>
       <c r="G79" s="3">
@@ -3524,16 +3527,16 @@
       <c r="B80" s="2">
         <v>611</v>
       </c>
-      <c r="C80" s="7">
+      <c r="C80" s="8">
         <v>309</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D80" s="7">
         <v>255</v>
       </c>
-      <c r="E80" s="7">
+      <c r="E80" s="9">
         <v>831</v>
       </c>
-      <c r="F80" s="7">
+      <c r="F80" s="9">
         <v>9083</v>
       </c>
       <c r="G80" s="3">
@@ -3562,16 +3565,16 @@
       <c r="B81" s="2">
         <v>611</v>
       </c>
-      <c r="C81" s="7">
+      <c r="C81" s="8">
         <v>309</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D81" s="7">
         <v>255</v>
       </c>
-      <c r="E81" s="7">
+      <c r="E81" s="9">
         <v>831</v>
       </c>
-      <c r="F81" s="7">
+      <c r="F81" s="9">
         <v>9084</v>
       </c>
       <c r="G81" s="3">
@@ -3600,16 +3603,16 @@
       <c r="B82" s="2">
         <v>611</v>
       </c>
-      <c r="C82" s="7">
+      <c r="C82" s="8">
         <v>309</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D82" s="7">
         <v>255</v>
       </c>
-      <c r="E82" s="7">
+      <c r="E82" s="9">
         <v>831</v>
       </c>
-      <c r="F82" s="7">
+      <c r="F82" s="9">
         <v>9086</v>
       </c>
       <c r="G82" s="3">
@@ -3638,16 +3641,16 @@
       <c r="B83" s="2">
         <v>611</v>
       </c>
-      <c r="C83" s="7">
+      <c r="C83" s="8">
         <v>310</v>
       </c>
-      <c r="D83" s="2">
+      <c r="D83" s="7">
         <v>255</v>
       </c>
-      <c r="E83" s="7">
+      <c r="E83" s="9">
         <v>836</v>
       </c>
-      <c r="F83" s="7">
+      <c r="F83" s="9">
         <v>9090</v>
       </c>
       <c r="G83" s="3">
@@ -3676,16 +3679,16 @@
       <c r="B84" s="2">
         <v>611</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C84" s="8">
         <v>310</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D84" s="7">
         <v>255</v>
       </c>
-      <c r="E84" s="7">
+      <c r="E84" s="9">
         <v>839</v>
       </c>
-      <c r="F84" s="7">
+      <c r="F84" s="9">
         <v>9095</v>
       </c>
       <c r="G84" s="3">
@@ -3714,16 +3717,16 @@
       <c r="B85" s="2">
         <v>612</v>
       </c>
-      <c r="C85" s="7">
+      <c r="C85" s="8">
         <v>310</v>
       </c>
-      <c r="D85" s="2">
+      <c r="D85" s="7">
         <v>255</v>
       </c>
-      <c r="E85" s="7">
+      <c r="E85" s="9">
         <v>839</v>
       </c>
-      <c r="F85" s="7">
+      <c r="F85" s="9">
         <v>9101</v>
       </c>
       <c r="G85" s="3">
@@ -3752,16 +3755,16 @@
       <c r="B86" s="2">
         <v>613</v>
       </c>
-      <c r="C86" s="7">
+      <c r="C86" s="8">
         <v>310</v>
       </c>
-      <c r="D86" s="2">
+      <c r="D86" s="7">
         <v>255</v>
       </c>
-      <c r="E86" s="7">
+      <c r="E86" s="9">
         <v>840</v>
       </c>
-      <c r="F86" s="7">
+      <c r="F86" s="9">
         <v>9111</v>
       </c>
       <c r="G86" s="3">
@@ -3790,16 +3793,16 @@
       <c r="B87" s="2">
         <v>613</v>
       </c>
-      <c r="C87" s="7">
+      <c r="C87" s="8">
         <v>310</v>
       </c>
-      <c r="D87" s="2">
+      <c r="D87" s="7">
         <v>255</v>
       </c>
-      <c r="E87" s="7">
+      <c r="E87" s="9">
         <v>842</v>
       </c>
-      <c r="F87" s="7">
+      <c r="F87" s="9">
         <v>9118</v>
       </c>
       <c r="G87" s="3">
@@ -3828,16 +3831,16 @@
       <c r="B88" s="2">
         <v>613</v>
       </c>
-      <c r="C88" s="7">
+      <c r="C88" s="8">
         <v>310</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D88" s="7">
         <v>255</v>
       </c>
-      <c r="E88" s="7">
+      <c r="E88" s="9">
         <v>842</v>
       </c>
-      <c r="F88" s="7">
+      <c r="F88" s="9">
         <v>9118</v>
       </c>
       <c r="G88" s="3">
@@ -3866,16 +3869,16 @@
       <c r="B89" s="2">
         <v>613</v>
       </c>
-      <c r="C89" s="7">
+      <c r="C89" s="8">
         <v>310</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D89" s="7">
         <v>255</v>
       </c>
-      <c r="E89" s="7">
+      <c r="E89" s="9">
         <v>844</v>
       </c>
-      <c r="F89" s="7">
+      <c r="F89" s="9">
         <v>9118</v>
       </c>
       <c r="G89" s="3">
@@ -3904,16 +3907,16 @@
       <c r="B90" s="2">
         <v>613</v>
       </c>
-      <c r="C90" s="7">
+      <c r="C90" s="8">
         <v>310</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90" s="7">
         <v>255</v>
       </c>
-      <c r="E90" s="7">
+      <c r="E90" s="9">
         <v>844</v>
       </c>
-      <c r="F90" s="7">
+      <c r="F90" s="9">
         <v>9122</v>
       </c>
       <c r="G90" s="3">
@@ -3942,16 +3945,16 @@
       <c r="B91" s="2">
         <v>614</v>
       </c>
-      <c r="C91" s="7">
+      <c r="C91" s="8">
         <v>311</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="7">
         <v>255</v>
       </c>
-      <c r="E91" s="7">
+      <c r="E91" s="9">
         <v>847</v>
       </c>
-      <c r="F91" s="7">
+      <c r="F91" s="9">
         <v>9128</v>
       </c>
       <c r="G91" s="3">
@@ -3980,16 +3983,16 @@
       <c r="B92" s="2">
         <v>615</v>
       </c>
-      <c r="C92" s="7">
+      <c r="C92" s="8">
         <v>312</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D92" s="7">
         <v>255</v>
       </c>
-      <c r="E92" s="7">
+      <c r="E92" s="9">
         <v>847</v>
       </c>
-      <c r="F92" s="7">
+      <c r="F92" s="9">
         <v>9134</v>
       </c>
       <c r="G92" s="3">
@@ -4018,16 +4021,16 @@
       <c r="B93" s="2">
         <v>615</v>
       </c>
-      <c r="C93" s="7">
+      <c r="C93" s="8">
         <v>312</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D93" s="7">
         <v>255</v>
       </c>
-      <c r="E93" s="7">
+      <c r="E93" s="9">
         <v>848</v>
       </c>
-      <c r="F93" s="7">
+      <c r="F93" s="9">
         <v>9141</v>
       </c>
       <c r="G93" s="3">
@@ -4056,16 +4059,16 @@
       <c r="B94" s="2">
         <v>615</v>
       </c>
-      <c r="C94" s="7">
+      <c r="C94" s="8">
         <v>312</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D94" s="7">
         <v>255</v>
       </c>
-      <c r="E94" s="7">
+      <c r="E94" s="9">
         <v>852</v>
       </c>
-      <c r="F94" s="7">
+      <c r="F94" s="9">
         <v>9148</v>
       </c>
       <c r="G94" s="3">
@@ -4094,16 +4097,16 @@
       <c r="B95" s="2">
         <v>615</v>
       </c>
-      <c r="C95" s="7">
+      <c r="C95" s="8">
         <v>312</v>
       </c>
-      <c r="D95" s="2">
+      <c r="D95" s="7">
         <v>255</v>
       </c>
-      <c r="E95" s="7">
+      <c r="E95" s="9">
         <v>856</v>
       </c>
-      <c r="F95" s="7">
+      <c r="F95" s="9">
         <v>9141</v>
       </c>
       <c r="G95" s="3">
@@ -4132,16 +4135,16 @@
       <c r="B96" s="2">
         <v>616</v>
       </c>
-      <c r="C96" s="7">
+      <c r="C96" s="8">
         <v>312</v>
       </c>
-      <c r="D96" s="2">
+      <c r="D96" s="7">
         <v>256</v>
       </c>
-      <c r="E96" s="7">
+      <c r="E96" s="9">
         <v>859</v>
       </c>
-      <c r="F96" s="7">
+      <c r="F96" s="9">
         <v>9148</v>
       </c>
       <c r="G96" s="3">
@@ -4170,16 +4173,16 @@
       <c r="B97" s="2">
         <v>616</v>
       </c>
-      <c r="C97" s="7">
+      <c r="C97" s="8">
         <v>313</v>
       </c>
-      <c r="D97" s="2">
+      <c r="D97" s="7">
         <v>256</v>
       </c>
-      <c r="E97" s="7">
+      <c r="E97" s="9">
         <v>861</v>
       </c>
-      <c r="F97" s="7">
+      <c r="F97" s="9">
         <v>9156</v>
       </c>
       <c r="G97" s="3">
@@ -4208,16 +4211,16 @@
       <c r="B98" s="2">
         <v>616</v>
       </c>
-      <c r="C98" s="7">
+      <c r="C98" s="8">
         <v>313</v>
       </c>
-      <c r="D98" s="2">
+      <c r="D98" s="7">
         <v>256</v>
       </c>
-      <c r="E98" s="7">
+      <c r="E98" s="9">
         <v>863</v>
       </c>
-      <c r="F98" s="7">
+      <c r="F98" s="9">
         <v>9168</v>
       </c>
       <c r="G98" s="3">
@@ -4246,16 +4249,16 @@
       <c r="B99" s="2">
         <v>617</v>
       </c>
-      <c r="C99" s="7">
+      <c r="C99" s="8">
         <v>313</v>
       </c>
-      <c r="D99" s="2">
+      <c r="D99" s="7">
         <v>256</v>
       </c>
-      <c r="E99" s="7">
+      <c r="E99" s="9">
         <v>863</v>
       </c>
-      <c r="F99" s="7">
+      <c r="F99" s="9">
         <v>9175</v>
       </c>
       <c r="G99" s="3">
@@ -4284,16 +4287,16 @@
       <c r="B100" s="2">
         <v>617</v>
       </c>
-      <c r="C100" s="7">
+      <c r="C100" s="8">
         <v>313</v>
       </c>
-      <c r="D100" s="2">
+      <c r="D100" s="7">
         <v>256</v>
       </c>
-      <c r="E100" s="7">
+      <c r="E100" s="9">
         <v>864</v>
       </c>
-      <c r="F100" s="7">
+      <c r="F100" s="9">
         <v>9183</v>
       </c>
       <c r="G100" s="3">
@@ -4322,16 +4325,16 @@
       <c r="B101" s="2">
         <v>617</v>
       </c>
-      <c r="C101" s="7">
+      <c r="C101" s="8">
         <v>313</v>
       </c>
-      <c r="D101" s="2">
+      <c r="D101" s="7">
         <v>256</v>
       </c>
-      <c r="E101" s="7">
+      <c r="E101" s="9">
         <v>866</v>
       </c>
-      <c r="F101" s="7">
+      <c r="F101" s="9">
         <v>9195</v>
       </c>
       <c r="G101" s="3">
@@ -4360,16 +4363,16 @@
       <c r="B102" s="2">
         <v>617</v>
       </c>
-      <c r="C102" s="7">
+      <c r="C102" s="8">
         <v>313</v>
       </c>
-      <c r="D102" s="2">
+      <c r="D102" s="7">
         <v>256</v>
       </c>
-      <c r="E102" s="7">
+      <c r="E102" s="9">
         <v>870</v>
       </c>
-      <c r="F102" s="7">
+      <c r="F102" s="9">
         <v>9196</v>
       </c>
       <c r="G102" s="3">
@@ -4398,16 +4401,16 @@
       <c r="B103" s="2">
         <v>620</v>
       </c>
-      <c r="C103" s="7">
+      <c r="C103" s="8">
         <v>313</v>
       </c>
-      <c r="D103" s="2">
+      <c r="D103" s="7">
         <v>256</v>
       </c>
-      <c r="E103" s="7">
+      <c r="E103" s="9">
         <v>872</v>
       </c>
-      <c r="F103" s="7">
+      <c r="F103" s="9">
         <v>9197</v>
       </c>
       <c r="G103" s="3">
@@ -4436,16 +4439,16 @@
       <c r="B104" s="2">
         <v>621</v>
       </c>
-      <c r="C104" s="7">
+      <c r="C104" s="8">
         <v>313</v>
       </c>
-      <c r="D104" s="2">
+      <c r="D104" s="7">
         <v>256</v>
       </c>
-      <c r="E104" s="7">
+      <c r="E104" s="9">
         <v>873</v>
       </c>
-      <c r="F104" s="7">
+      <c r="F104" s="9">
         <v>9201</v>
       </c>
       <c r="G104" s="3">
@@ -4474,16 +4477,16 @@
       <c r="B105" s="2">
         <v>621</v>
       </c>
-      <c r="C105" s="7">
+      <c r="C105" s="8">
         <v>313</v>
       </c>
-      <c r="D105" s="2">
+      <c r="D105" s="7">
         <v>256</v>
       </c>
-      <c r="E105" s="7">
+      <c r="E105" s="9">
         <v>873</v>
       </c>
-      <c r="F105" s="7">
+      <c r="F105" s="9">
         <v>9207</v>
       </c>
       <c r="G105" s="3">
@@ -4512,16 +4515,16 @@
       <c r="B106" s="2">
         <v>621</v>
       </c>
-      <c r="C106" s="7">
+      <c r="C106" s="8">
         <v>313</v>
       </c>
-      <c r="D106" s="2">
+      <c r="D106" s="7">
         <v>257</v>
       </c>
-      <c r="E106" s="7">
+      <c r="E106" s="9">
         <v>875</v>
       </c>
-      <c r="F106" s="7">
+      <c r="F106" s="9">
         <v>9211</v>
       </c>
       <c r="G106" s="3">
@@ -4550,16 +4553,16 @@
       <c r="B107" s="2">
         <v>621</v>
       </c>
-      <c r="C107" s="7">
+      <c r="C107" s="8">
         <v>313</v>
       </c>
-      <c r="D107" s="2">
+      <c r="D107" s="7">
         <v>261</v>
       </c>
-      <c r="E107" s="7">
+      <c r="E107" s="9">
         <v>877</v>
       </c>
-      <c r="F107" s="7">
+      <c r="F107" s="9">
         <v>9225</v>
       </c>
       <c r="G107" s="3">
@@ -4588,16 +4591,16 @@
       <c r="B108" s="2">
         <v>621</v>
       </c>
-      <c r="C108" s="7">
+      <c r="C108" s="8">
         <v>313</v>
       </c>
-      <c r="D108" s="2">
+      <c r="D108" s="7">
         <v>261</v>
       </c>
-      <c r="E108" s="7">
+      <c r="E108" s="9">
         <v>880</v>
       </c>
-      <c r="F108" s="7">
+      <c r="F108" s="9">
         <v>9231</v>
       </c>
       <c r="G108" s="3">
@@ -4626,16 +4629,16 @@
       <c r="B109" s="2">
         <v>621</v>
       </c>
-      <c r="C109" s="7">
+      <c r="C109" s="8">
         <v>313</v>
       </c>
-      <c r="D109" s="2">
+      <c r="D109" s="7">
         <v>261</v>
       </c>
-      <c r="E109" s="7">
+      <c r="E109" s="9">
         <v>881</v>
       </c>
-      <c r="F109" s="7">
+      <c r="F109" s="9">
         <v>9231</v>
       </c>
       <c r="G109" s="3">
@@ -4664,16 +4667,16 @@
       <c r="B110" s="2">
         <v>621</v>
       </c>
-      <c r="C110" s="7">
+      <c r="C110" s="8">
         <v>314</v>
       </c>
-      <c r="D110" s="2">
+      <c r="D110" s="7">
         <v>261</v>
       </c>
-      <c r="E110" s="7">
+      <c r="E110" s="9">
         <v>882</v>
       </c>
-      <c r="F110" s="7">
+      <c r="F110" s="9">
         <v>9232</v>
       </c>
       <c r="G110" s="3">
@@ -4702,16 +4705,16 @@
       <c r="B111" s="2">
         <v>621</v>
       </c>
-      <c r="C111" s="7">
+      <c r="C111" s="8">
         <v>314</v>
       </c>
-      <c r="D111" s="2">
+      <c r="D111" s="7">
         <v>262</v>
       </c>
-      <c r="E111" s="7">
+      <c r="E111" s="9">
         <v>883</v>
       </c>
-      <c r="F111" s="7">
+      <c r="F111" s="9">
         <v>9236</v>
       </c>
       <c r="G111" s="3">
@@ -4740,16 +4743,16 @@
       <c r="B112" s="2">
         <v>621</v>
       </c>
-      <c r="C112" s="7">
+      <c r="C112" s="8">
         <v>314</v>
       </c>
-      <c r="D112" s="2">
+      <c r="D112" s="7">
         <v>262</v>
       </c>
-      <c r="E112" s="7">
+      <c r="E112" s="9">
         <v>884</v>
       </c>
-      <c r="F112" s="7">
+      <c r="F112" s="9">
         <v>9243</v>
       </c>
       <c r="G112" s="3">
@@ -4778,16 +4781,16 @@
       <c r="B113" s="2">
         <v>621</v>
       </c>
-      <c r="C113" s="7">
+      <c r="C113" s="8">
         <v>314</v>
       </c>
-      <c r="D113" s="2">
+      <c r="D113" s="7">
         <v>264</v>
       </c>
-      <c r="E113" s="7">
+      <c r="E113" s="9">
         <v>886</v>
       </c>
-      <c r="F113" s="7">
+      <c r="F113" s="9">
         <v>9253</v>
       </c>
       <c r="G113" s="3">
@@ -4816,16 +4819,16 @@
       <c r="B114" s="2">
         <v>621</v>
       </c>
-      <c r="C114" s="7">
+      <c r="C114" s="8">
         <v>314</v>
       </c>
-      <c r="D114" s="2">
+      <c r="D114" s="7">
         <v>264</v>
       </c>
-      <c r="E114" s="7">
+      <c r="E114" s="9">
         <v>888</v>
       </c>
-      <c r="F114" s="7">
+      <c r="F114" s="9">
         <v>9260</v>
       </c>
       <c r="G114" s="3">
@@ -4854,16 +4857,16 @@
       <c r="B115" s="2">
         <v>622</v>
       </c>
-      <c r="C115" s="7">
+      <c r="C115" s="8">
         <v>314</v>
       </c>
-      <c r="D115" s="2">
+      <c r="D115" s="7">
         <v>264</v>
       </c>
-      <c r="E115" s="7">
+      <c r="E115" s="9">
         <v>890</v>
       </c>
-      <c r="F115" s="7">
+      <c r="F115" s="9">
         <v>9267</v>
       </c>
       <c r="G115" s="3">
@@ -4892,16 +4895,16 @@
       <c r="B116" s="2">
         <v>622</v>
       </c>
-      <c r="C116" s="7">
+      <c r="C116" s="8">
         <v>314</v>
       </c>
-      <c r="D116" s="2">
+      <c r="D116" s="7">
         <v>264</v>
       </c>
-      <c r="E116" s="7">
+      <c r="E116" s="9">
         <v>893</v>
       </c>
-      <c r="F116" s="7">
+      <c r="F116" s="9">
         <v>9269</v>
       </c>
       <c r="G116" s="3">
@@ -4930,16 +4933,16 @@
       <c r="B117" s="2">
         <v>623</v>
       </c>
-      <c r="C117" s="7">
+      <c r="C117" s="8">
         <v>314</v>
       </c>
-      <c r="D117" s="2">
+      <c r="D117" s="7">
         <v>264</v>
       </c>
-      <c r="E117" s="7">
+      <c r="E117" s="9">
         <v>895</v>
       </c>
-      <c r="F117" s="7">
+      <c r="F117" s="9">
         <v>9272</v>
       </c>
       <c r="G117" s="3">
@@ -4968,16 +4971,16 @@
       <c r="B118" s="2">
         <v>623</v>
       </c>
-      <c r="C118" s="7">
+      <c r="C118" s="8">
         <v>314</v>
       </c>
-      <c r="D118" s="2">
+      <c r="D118" s="7">
         <v>264</v>
       </c>
-      <c r="E118" s="7">
+      <c r="E118" s="9">
         <v>897</v>
       </c>
-      <c r="F118" s="7">
+      <c r="F118" s="9">
         <v>9277</v>
       </c>
       <c r="G118" s="3">
@@ -5006,16 +5009,16 @@
       <c r="B119" s="2">
         <v>623</v>
       </c>
-      <c r="C119" s="7">
+      <c r="C119" s="8">
         <v>314</v>
       </c>
-      <c r="D119" s="2">
+      <c r="D119" s="7">
         <v>264</v>
       </c>
-      <c r="E119" s="7">
+      <c r="E119" s="9">
         <v>902</v>
       </c>
-      <c r="F119" s="7">
+      <c r="F119" s="9">
         <v>9280</v>
       </c>
       <c r="G119" s="3">
@@ -5044,16 +5047,16 @@
       <c r="B120" s="2">
         <v>624</v>
       </c>
-      <c r="C120" s="7">
+      <c r="C120" s="8">
         <v>314</v>
       </c>
-      <c r="D120" s="2">
+      <c r="D120" s="7">
         <v>264</v>
       </c>
-      <c r="E120" s="7">
+      <c r="E120" s="9">
         <v>902</v>
       </c>
-      <c r="F120" s="7">
+      <c r="F120" s="9">
         <v>9285</v>
       </c>
       <c r="G120" s="3">
@@ -5082,16 +5085,16 @@
       <c r="B121" s="2">
         <v>624</v>
       </c>
-      <c r="C121" s="7">
+      <c r="C121" s="8">
         <v>314</v>
       </c>
-      <c r="D121" s="2">
+      <c r="D121" s="7">
         <v>264</v>
       </c>
-      <c r="E121" s="7">
+      <c r="E121" s="9">
         <v>902</v>
       </c>
-      <c r="F121" s="7">
+      <c r="F121" s="9">
         <v>9288</v>
       </c>
       <c r="G121" s="3">
@@ -5120,16 +5123,16 @@
       <c r="B122" s="2">
         <v>624</v>
       </c>
-      <c r="C122" s="7">
+      <c r="C122" s="8">
         <v>314</v>
       </c>
-      <c r="D122" s="2">
+      <c r="D122" s="7">
         <v>264</v>
       </c>
-      <c r="E122" s="7">
+      <c r="E122" s="9">
         <v>902</v>
       </c>
-      <c r="F122" s="7">
+      <c r="F122" s="9">
         <v>9289</v>
       </c>
       <c r="G122" s="3">
@@ -5158,16 +5161,16 @@
       <c r="B123" s="2">
         <v>624</v>
       </c>
-      <c r="C123" s="7">
+      <c r="C123" s="8">
         <v>314</v>
       </c>
-      <c r="D123" s="2">
+      <c r="D123" s="7">
         <v>264</v>
       </c>
-      <c r="E123" s="7">
+      <c r="E123" s="9">
         <v>903</v>
       </c>
-      <c r="F123" s="7">
+      <c r="F123" s="9">
         <v>9295</v>
       </c>
       <c r="G123" s="3">
@@ -5196,16 +5199,16 @@
       <c r="B124" s="2">
         <v>624</v>
       </c>
-      <c r="C124" s="7">
+      <c r="C124" s="8">
         <v>314</v>
       </c>
-      <c r="D124" s="2">
+      <c r="D124" s="7">
         <v>264</v>
       </c>
-      <c r="E124" s="7">
+      <c r="E124" s="9">
         <v>903</v>
       </c>
-      <c r="F124" s="7">
+      <c r="F124" s="9">
         <v>9298</v>
       </c>
       <c r="G124" s="3">

</xml_diff>